<commit_message>
Mini changes to GanttChart
</commit_message>
<xml_diff>
--- a/Workplan/GanttChart.xlsx
+++ b/Workplan/GanttChart.xlsx
@@ -759,7 +759,7 @@
       <pane xSplit="6" ySplit="8" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1560,7 +1560,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="H10" s="6"/>
     </row>
@@ -1579,7 +1579,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="3">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="H11" s="4"/>
     </row>
@@ -1598,7 +1598,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1660,7 +1660,7 @@
         <v>3</v>
       </c>
       <c r="E15" s="3">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K15" s="15"/>
     </row>
@@ -1669,18 +1669,19 @@
         <v>10</v>
       </c>
       <c r="B16" s="10">
-        <v>42506</v>
+        <v>42499</v>
       </c>
       <c r="C16" s="10">
         <v>42517</v>
       </c>
       <c r="D16" s="21">
         <f t="shared" si="3"/>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E16" s="3">
         <v>0</v>
       </c>
+      <c r="K16" s="4"/>
       <c r="L16" s="4"/>
       <c r="M16" s="4"/>
     </row>

</xml_diff>

<commit_message>
Updated gantt chart (we are done with the list) and re-arranged some documents.
</commit_message>
<xml_diff>
--- a/Workplan/GanttChart.xlsx
+++ b/Workplan/GanttChart.xlsx
@@ -756,10 +756,10 @@
   <dimension ref="A1:BO63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="8" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="8" topLeftCell="J31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1826,7 +1826,7 @@
         <v>51</v>
       </c>
       <c r="E23" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>

</xml_diff>

<commit_message>
Workplan updated with the completed tasks
</commit_message>
<xml_diff>
--- a/Workplan/GanttChart.xlsx
+++ b/Workplan/GanttChart.xlsx
@@ -416,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -451,6 +451,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,10 +759,10 @@
   <dimension ref="A1:BO63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="6" ySplit="8" topLeftCell="J31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="8" topLeftCell="AX46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomRight" activeCell="B62" sqref="B62:C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -768,7 +771,7 @@
     <col min="2" max="3" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="3" customWidth="1"/>
     <col min="7" max="7" width="5.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -1338,7 +1341,7 @@
       <c r="E8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="24" t="s">
         <v>43</v>
       </c>
       <c r="G8" s="11">
@@ -2135,14 +2138,14 @@
         <v>24</v>
       </c>
       <c r="B36" s="10">
-        <v>42661</v>
+        <v>42692</v>
       </c>
       <c r="C36" s="10">
         <v>42692</v>
       </c>
       <c r="D36" s="21">
         <f t="shared" si="3"/>
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E36" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
Updated our GanttChart, just because...
</commit_message>
<xml_diff>
--- a/Workplan/GanttChart.xlsx
+++ b/Workplan/GanttChart.xlsx
@@ -740,10 +740,10 @@
   <dimension ref="A1:BO63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="8" topLeftCell="G9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="8" topLeftCell="G24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1063,7 +1063,7 @@
       <c r="B7" s="5"/>
       <c r="D7" s="25">
         <f>SUMPRODUCT(D9:D62,E9:E62)/SUM(D9:D62)</f>
-        <v>22.220064724919094</v>
+        <v>30.414239482200646</v>
       </c>
       <c r="F7" t="s">
         <v>39</v>
@@ -1670,7 +1670,7 @@
         <v>18</v>
       </c>
       <c r="E16" s="3">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
@@ -1691,7 +1691,7 @@
         <v>18</v>
       </c>
       <c r="E17" s="3">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="J17" s="14"/>
       <c r="K17" s="7"/>
@@ -1757,7 +1757,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -1777,7 +1777,7 @@
         <v>9</v>
       </c>
       <c r="E21" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N21" s="4"/>
       <c r="O21" s="16"/>
@@ -1797,7 +1797,7 @@
         <v>16</v>
       </c>
       <c r="E22" s="3">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
@@ -1845,7 +1845,7 @@
         <v>9</v>
       </c>
       <c r="E24" s="3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -1865,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="3">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="O25" s="4"/>
     </row>
@@ -1884,7 +1884,7 @@
         <v>86</v>
       </c>
       <c r="E26" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>51</v>
@@ -1918,7 +1918,7 @@
         <v>86</v>
       </c>
       <c r="E27" s="3">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
@@ -1950,7 +1950,7 @@
         <v>86</v>
       </c>
       <c r="E28" s="3">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
@@ -1982,7 +1982,7 @@
         <v>42</v>
       </c>
       <c r="E29" s="3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W29" s="1"/>
       <c r="X29" s="6"/>

</xml_diff>

<commit_message>
Updated worlplan with summer's work
</commit_message>
<xml_diff>
--- a/Workplan/GanttChart.xlsx
+++ b/Workplan/GanttChart.xlsx
@@ -679,10 +679,10 @@
   <dimension ref="A1:BO63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="8" topLeftCell="Z27" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="8" topLeftCell="T29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomRight" activeCell="AD30" sqref="AD30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1002,7 +1002,7 @@
       <c r="B7" s="5"/>
       <c r="D7" s="25">
         <f>SUMPRODUCT(D9:D62,E9:E62)/SUM(D9:D62)/100</f>
-        <v>0.35702265372168285</v>
+        <v>0.3964401294498382</v>
       </c>
       <c r="F7" t="s">
         <v>39</v>
@@ -1823,7 +1823,7 @@
         <v>86</v>
       </c>
       <c r="E26" s="3">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="P26" s="1" t="s">
         <v>51</v>
@@ -1857,7 +1857,7 @@
         <v>86</v>
       </c>
       <c r="E27" s="3">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="P27" s="6"/>
       <c r="Q27" s="6"/>
@@ -1889,7 +1889,7 @@
         <v>86</v>
       </c>
       <c r="E28" s="3">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="P28" s="6"/>
       <c r="Q28" s="6"/>
@@ -1921,7 +1921,7 @@
         <v>42</v>
       </c>
       <c r="E29" s="3">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="W29" s="1"/>
       <c r="X29" s="6"/>
@@ -1984,7 +1984,7 @@
         <v>4</v>
       </c>
       <c r="E32" s="3">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="AD32" s="4"/>
     </row>

</xml_diff>